<commit_message>
update metrics and analysis
</commit_message>
<xml_diff>
--- a/oops/oops-summary.xlsx
+++ b/oops/oops-summary.xlsx
@@ -5,16 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesualdo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesualdo/git/OntoGenixEvaluation/oops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3156B33-31E1-6545-B115-9A5E31AF1FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A631E6-9D2F-D145-BBFE-FC3210DC7A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="description of pitfalls" sheetId="5" r:id="rId2"/>
+    <sheet name="pitfalls-all" sheetId="1" r:id="rId1"/>
+    <sheet name="pitfalls-human" sheetId="6" r:id="rId2"/>
+    <sheet name="pitfalls-ontogenix" sheetId="7" r:id="rId3"/>
+    <sheet name="description of pitfalls" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="68">
   <si>
     <t>AIRLINES</t>
   </si>
@@ -144,9 +146,6 @@
     <t>P39</t>
   </si>
   <si>
-    <t>PITFALL</t>
-  </si>
-  <si>
     <t>DEFINITION</t>
   </si>
   <si>
@@ -214,13 +213,40 @@
   </si>
   <si>
     <t>Ambiguous namespace</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>Pitfall</t>
+  </si>
+  <si>
+    <t>Airlines</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>BigBasket</t>
+  </si>
+  <si>
+    <t>Brazilian</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>E-commerce</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -233,6 +259,17 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -291,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -308,10 +345,31 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,40 +590,40 @@
   </sheetPr>
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="1"/>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="9" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="12"/>
+      <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="12"/>
+      <c r="I1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="10"/>
-      <c r="M1" s="9" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="12"/>
+      <c r="M1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="11" t="s">
+      <c r="N1" s="12"/>
+      <c r="O1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="10"/>
+      <c r="P1" s="12"/>
       <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1566,13 +1624,1133 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBFCF776-BA97-7143-8E8E-1186C0A3E69A}">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B1" s="1"/>
+      <c r="C1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3">
+        <f t="shared" ref="C2:H2" si="0">COUNT(C3:C21)</f>
+        <v>4</v>
+      </c>
+      <c r="D2" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E2" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G2" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H2" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I2" s="3">
+        <f>SUM(I3:I21)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" ref="I3:I21" si="1">COUNT(C3,D3,E3,F3,G3,H3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" ref="C23:I23" si="2">SUM(C10,C14,C19,C21)</f>
+        <v>2</v>
+      </c>
+      <c r="D23" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F23" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H23" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" ref="C24:I24" si="3">SUM(C7,C8,C13,C16,C17,C20)</f>
+        <v>1</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E24" s="7">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F24" s="7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G24" s="7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="H24" s="7">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I24" s="7">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="8">
+        <f t="shared" ref="C25:I25" si="4">SUM(C3:C6,C9,C11,C12,C15,C18)</f>
+        <v>1</v>
+      </c>
+      <c r="D25" s="8">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F25" s="8">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="G25" s="8">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="H25" s="8">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="I25" s="8">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561C338A-6F90-2A42-8E23-A6F92E12D949}">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="14">
+        <v>13</v>
+      </c>
+      <c r="D2" s="14">
+        <v>7</v>
+      </c>
+      <c r="E2" s="14">
+        <v>8</v>
+      </c>
+      <c r="F2" s="14">
+        <v>9</v>
+      </c>
+      <c r="G2" s="14">
+        <v>12</v>
+      </c>
+      <c r="H2" s="14">
+        <v>10</v>
+      </c>
+      <c r="I2" s="14">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="14">
+        <v>1</v>
+      </c>
+      <c r="G3" s="14">
+        <v>1</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14">
+        <v>1</v>
+      </c>
+      <c r="F6" s="14">
+        <v>1</v>
+      </c>
+      <c r="G6" s="14">
+        <v>1</v>
+      </c>
+      <c r="H6" s="14">
+        <v>1</v>
+      </c>
+      <c r="I6" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1</v>
+      </c>
+      <c r="F7" s="14">
+        <v>1</v>
+      </c>
+      <c r="G7" s="14">
+        <v>1</v>
+      </c>
+      <c r="H7" s="14">
+        <v>1</v>
+      </c>
+      <c r="I7" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="14">
+        <v>1</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1</v>
+      </c>
+      <c r="G9" s="14">
+        <v>1</v>
+      </c>
+      <c r="H9" s="14">
+        <v>1</v>
+      </c>
+      <c r="I9" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="14">
+        <v>1</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="14">
+        <v>1</v>
+      </c>
+      <c r="H12" s="14">
+        <v>1</v>
+      </c>
+      <c r="I12" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="14">
+        <v>1</v>
+      </c>
+      <c r="H13" s="18"/>
+      <c r="I13" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="14">
+        <v>1</v>
+      </c>
+      <c r="H14" s="14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="14">
+        <v>1</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="14">
+        <v>1</v>
+      </c>
+      <c r="G16" s="14">
+        <v>1</v>
+      </c>
+      <c r="H16" s="14">
+        <v>1</v>
+      </c>
+      <c r="I16" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14">
+        <v>1</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="14">
+        <v>1</v>
+      </c>
+      <c r="H17" s="14">
+        <v>1</v>
+      </c>
+      <c r="I17" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1</v>
+      </c>
+      <c r="D18" s="14">
+        <v>1</v>
+      </c>
+      <c r="E18" s="14">
+        <v>1</v>
+      </c>
+      <c r="F18" s="14">
+        <v>1</v>
+      </c>
+      <c r="G18" s="14">
+        <v>1</v>
+      </c>
+      <c r="H18" s="14">
+        <v>1</v>
+      </c>
+      <c r="I18" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="14">
+        <v>1</v>
+      </c>
+      <c r="D20" s="14">
+        <v>1</v>
+      </c>
+      <c r="E20" s="14">
+        <v>1</v>
+      </c>
+      <c r="F20" s="14">
+        <v>1</v>
+      </c>
+      <c r="G20" s="14">
+        <v>1</v>
+      </c>
+      <c r="H20" s="14">
+        <v>1</v>
+      </c>
+      <c r="I20" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="14">
+        <v>1</v>
+      </c>
+      <c r="D21" s="14">
+        <v>1</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="14">
+        <v>1</v>
+      </c>
+      <c r="G21" s="14">
+        <v>1</v>
+      </c>
+      <c r="H21" s="14">
+        <v>1</v>
+      </c>
+      <c r="I21" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+    </row>
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="18"/>
+      <c r="B23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="20">
+        <v>3</v>
+      </c>
+      <c r="D23" s="20">
+        <v>1</v>
+      </c>
+      <c r="E23" s="20">
+        <v>1</v>
+      </c>
+      <c r="F23" s="20">
+        <v>2</v>
+      </c>
+      <c r="G23" s="20">
+        <v>2</v>
+      </c>
+      <c r="H23" s="20">
+        <v>2</v>
+      </c>
+      <c r="I23" s="20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="18"/>
+      <c r="B24" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="21">
+        <v>4</v>
+      </c>
+      <c r="D24" s="21">
+        <v>3</v>
+      </c>
+      <c r="E24" s="21">
+        <v>3</v>
+      </c>
+      <c r="F24" s="21">
+        <v>3</v>
+      </c>
+      <c r="G24" s="21">
+        <v>5</v>
+      </c>
+      <c r="H24" s="21">
+        <v>4</v>
+      </c>
+      <c r="I24" s="21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="18"/>
+      <c r="B25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="22">
+        <v>6</v>
+      </c>
+      <c r="D25" s="22">
+        <v>3</v>
+      </c>
+      <c r="E25" s="22">
+        <v>4</v>
+      </c>
+      <c r="F25" s="22">
+        <v>4</v>
+      </c>
+      <c r="G25" s="22">
+        <v>5</v>
+      </c>
+      <c r="H25" s="22">
+        <v>4</v>
+      </c>
+      <c r="I25" s="22">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1581,10 +2759,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>13</v>
@@ -1595,10 +2773,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1606,10 +2784,10 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1617,10 +2795,10 @@
         <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1628,10 +2806,10 @@
         <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1639,10 +2817,10 @@
         <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1650,10 +2828,10 @@
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1661,10 +2839,10 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1672,10 +2850,10 @@
         <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1683,10 +2861,10 @@
         <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1694,10 +2872,10 @@
         <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1705,10 +2883,10 @@
         <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1716,10 +2894,10 @@
         <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1727,10 +2905,10 @@
         <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1738,10 +2916,10 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1749,10 +2927,10 @@
         <v>31</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1760,10 +2938,10 @@
         <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1771,10 +2949,10 @@
         <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1782,10 +2960,10 @@
         <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1793,10 +2971,10 @@
         <v>35</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>